<commit_message>
Added fp-category-cs codes for SPLASCH data, at least for connectathon.
</commit_message>
<xml_diff>
--- a/output/CodeSystem-fp-category-cs.xlsx
+++ b/output/CodeSystem-fp-category-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="141">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-19T12:58:34-04:00</t>
+    <t>2022-04-26T11:43:49-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -117,7 +117,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>19</t>
+    <t>33</t>
   </si>
   <si>
     <t>Level</t>
@@ -165,6 +165,42 @@
     <t>Functions of the senses, seeing, hearing, tasting and so on, as well as the sensation of pain.</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>seeing-and-related-functions</t>
+  </si>
+  <si>
+    <t>Seeing and related functions</t>
+  </si>
+  <si>
+    <t>Seeing and related functions.</t>
+  </si>
+  <si>
+    <t>hearing-and-vestibular-functions</t>
+  </si>
+  <si>
+    <t>Hearing and vestibular functions</t>
+  </si>
+  <si>
+    <t>Hearing and vestibular functions.</t>
+  </si>
+  <si>
+    <t>additional-sensory-functions</t>
+  </si>
+  <si>
+    <t>Additional sensory functions</t>
+  </si>
+  <si>
+    <t>Additional sensory functions.</t>
+  </si>
+  <si>
+    <t>pain</t>
+  </si>
+  <si>
+    <t>Pain</t>
+  </si>
+  <si>
     <t>voice-and-speech-functions</t>
   </si>
   <si>
@@ -192,6 +228,72 @@
     <t>Functions of ingestion, digestion and elimination, as well as functions involved in metabolism and the endocrine glands.</t>
   </si>
   <si>
+    <t>functions-related-to-the-digestive-system</t>
+  </si>
+  <si>
+    <t>Functions related to the digestive system</t>
+  </si>
+  <si>
+    <t>Functions related to the digestive system.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>ingestion-functions</t>
+  </si>
+  <si>
+    <t>Ingestion functions</t>
+  </si>
+  <si>
+    <t>Functions related to taking in and manipulating solids or liquids through the mouth into the body.</t>
+  </si>
+  <si>
+    <t>digestive-functions</t>
+  </si>
+  <si>
+    <t>Digestive functions</t>
+  </si>
+  <si>
+    <t>Functions of transporting food through the gastrointestinal tract, breakdown of food and absorption of nutrients.</t>
+  </si>
+  <si>
+    <t>assimilation-functions</t>
+  </si>
+  <si>
+    <t>Assimilation functions</t>
+  </si>
+  <si>
+    <t>Functions by which nutrients are converted into components of the living body.</t>
+  </si>
+  <si>
+    <t>defecation-functions</t>
+  </si>
+  <si>
+    <t>Defecation functions</t>
+  </si>
+  <si>
+    <t>Functions of elimination of wastes and undigested food as faeces and related functions.</t>
+  </si>
+  <si>
+    <t>weight-maintenance-functions</t>
+  </si>
+  <si>
+    <t>Weight maintenance functions</t>
+  </si>
+  <si>
+    <t>Functions of maintaining appropriate body weight, including weight gain during the developmental period.</t>
+  </si>
+  <si>
+    <t>sensations-associated-with-the-digestive-system</t>
+  </si>
+  <si>
+    <t>Sensations associated with the digestive system</t>
+  </si>
+  <si>
+    <t>Sensations arising from eating, drinking and related digestive functions.</t>
+  </si>
+  <si>
     <t>genitourinary-and-reproductive-functions</t>
   </si>
   <si>
@@ -253,6 +355,33 @@
   </si>
   <si>
     <t>General and specific features of communicating by language, signs and symbols, including receiving and producing messages, carrying on conversations, and using communication devices and techniques.</t>
+  </si>
+  <si>
+    <t>communication-receiving</t>
+  </si>
+  <si>
+    <t>Communication - receiving</t>
+  </si>
+  <si>
+    <t>Communication - receiving.</t>
+  </si>
+  <si>
+    <t>communication-producing</t>
+  </si>
+  <si>
+    <t>Communication - producing</t>
+  </si>
+  <si>
+    <t>Communication - producing.</t>
+  </si>
+  <si>
+    <t>conversation-and-use-of-communication-devices-and-techniques</t>
+  </si>
+  <si>
+    <t>Conversation and use of communication devices and techniques</t>
+  </si>
+  <si>
+    <t>Conversation and use of communication devices and techniques.</t>
   </si>
   <si>
     <t>mobility</t>
@@ -623,7 +752,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -687,55 +816,55 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>61</v>
@@ -771,7 +900,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s" s="2">
         <v>68</v>
@@ -785,7 +914,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s" s="2">
         <v>71</v>
@@ -799,86 +928,86 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19">
@@ -886,13 +1015,13 @@
         <v>43</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20">
@@ -900,13 +1029,209 @@
         <v>43</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="D22" t="s" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="D23" t="s" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="D27" t="s" s="2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="D30" t="s" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="D31" t="s" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="D33" t="s" s="2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="D34" t="s" s="2">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>